<commit_message>
add generator passwords different complexity
</commit_message>
<xml_diff>
--- a/MyPass/MyPass/1.xlsx
+++ b/MyPass/MyPass/1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Site</t>
   </si>
@@ -28,12 +28,6 @@
   </si>
   <si>
     <t>Passwords</t>
-  </si>
-  <si>
-    <t>www.1</t>
-  </si>
-  <si>
-    <t>ddfire</t>
   </si>
 </sst>
 </file>
@@ -351,7 +345,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="A1:D3"/>
@@ -370,17 +364,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add show DB passwords
</commit_message>
<xml_diff>
--- a/MyPass/MyPass/1.xlsx
+++ b/MyPass/MyPass/1.xlsx
@@ -19,7 +19,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Passwords</t>
+  </si>
+  <si>
+    <t>www.d</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Z.=QDH6AfP}E</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -335,14 +354,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add show pass fix open file
</commit_message>
<xml_diff>
--- a/MyPass/MyPass/1.xlsx
+++ b/MyPass/MyPass/1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Site</t>
   </si>
@@ -46,6 +46,21 @@
   </si>
   <si>
     <t>r&gt;=-x;M0</t>
+  </si>
+  <si>
+    <t>www.f</t>
+  </si>
+  <si>
+    <t>dima</t>
+  </si>
+  <si>
+    <t>LRvWxWSA</t>
+  </si>
+  <si>
+    <t>www.dima</t>
+  </si>
+  <si>
+    <t>zR{X7/9od7nF</t>
   </si>
 </sst>
 </file>
@@ -363,7 +378,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="A1:D3"/>
@@ -404,6 +419,28 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add inteface and class empty grafik fix
</commit_message>
<xml_diff>
--- a/MyPass/MyPass/1.xlsx
+++ b/MyPass/MyPass/1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Site</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>+{_9RI-wkw&gt;a+*fU</t>
+  </si>
+  <si>
+    <t>www.test</t>
+  </si>
+  <si>
+    <t>lena_dima</t>
+  </si>
+  <si>
+    <t>&amp;).A-O}\</t>
   </si>
 </sst>
 </file>
@@ -387,7 +396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="A1:D3"/>
@@ -461,6 +470,17 @@
         <v>16</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>